<commit_message>
updates trap data and metadata to have trap start, end
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_trap_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_trap_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ED4A53-CDAE-40F0-9D1D-8AFD4AA9CC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B1B52-2AD1-45B9-A59C-06D291EF1251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="530" windowWidth="20470" windowHeight="11390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="82">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -199,9 +199,6 @@
     <t>conductivity</t>
   </si>
   <si>
-    <t>waterTempUnit</t>
-  </si>
-  <si>
     <t>Lower Feather RST</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>Discharge measured at trap</t>
   </si>
   <si>
-    <t>Unit of water temperature recorded. Levels = c(NA, "Celsius", "Fahrenheit").</t>
-  </si>
-  <si>
     <t>Work that was done during visit to trap. Levels = c("Start trap &amp; begin trapping", "Continue trapping", "Unplanned restart", "End trapping", "Drive-by only", "Service/adjust/clean trap")</t>
   </si>
   <si>
@@ -257,6 +251,27 @@
   </si>
   <si>
     <t>2025-06-02 10:00:26</t>
+  </si>
+  <si>
+    <t>counterAtStart</t>
+  </si>
+  <si>
+    <t>Reading on the rotation counter at the start of the trap visit</t>
+  </si>
+  <si>
+    <t>trap_start_date</t>
+  </si>
+  <si>
+    <t>Start date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>trap_end_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>2025-06-02 09:45:50</t>
   </si>
 </sst>
 </file>
@@ -329,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,6 +388,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -670,7 +688,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -746,7 +764,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -784,7 +802,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -842,10 +860,10 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -863,16 +881,16 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>25</v>
@@ -886,10 +904,10 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -910,7 +928,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -948,7 +966,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
@@ -986,7 +1004,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1021,10 +1039,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -1051,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>7608</v>
+        <v>6150</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1069,10 +1087,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>32</v>
@@ -1087,7 +1105,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>35</v>
@@ -1099,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>5.6</v>
+        <v>7608</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1117,7 +1135,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>37</v>
@@ -1147,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="3">
-        <v>5.95</v>
+        <v>5.6</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1165,28 +1183,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5.95</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1203,38 +1231,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="3">
-        <v>32.409999999999997</v>
-      </c>
-      <c r="M15" s="3">
-        <v>51654</v>
-      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1251,10 +1269,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -1269,7 +1287,7 @@
         <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>35</v>
@@ -1278,10 +1296,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>32.409999999999997</v>
       </c>
       <c r="M16" s="3">
-        <v>1.4</v>
+        <v>51654</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1299,10 +1317,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1317,7 +1335,7 @@
         <v>32</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>35</v>
@@ -1326,10 +1344,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
       <c r="L17" s="3">
-        <v>5.0199999999999996</v>
+        <v>0</v>
       </c>
       <c r="M17" s="3">
-        <v>68.599999999999994</v>
+        <v>1.4</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1345,12 +1363,12 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>46</v>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>47</v>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>32</v>
@@ -1364,8 +1382,8 @@
       <c r="F18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>48</v>
+      <c r="G18" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>35</v>
@@ -1374,58 +1392,58 @@
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
       <c r="L18" s="3">
-        <v>0.73</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="M18" s="3">
-        <v>59.6</v>
+        <v>68.599999999999994</v>
       </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13">
-        <v>6.7900000000000002E-2</v>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3">
+        <v>0.73</v>
       </c>
-      <c r="M19" s="13">
-        <v>830</v>
+      <c r="M19" s="3">
+        <v>59.6</v>
       </c>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -1441,78 +1459,88 @@
       <c r="Y19" s="13"/>
       <c r="Z19" s="13"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13">
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="M20" s="13">
+        <v>830</v>
+      </c>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>77.900000000000006</v>
-      </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <v>77.900000000000006</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1528,19 +1556,35 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
+      <c r="A22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="L22" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1556,19 +1600,35 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
+      <c r="A23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="L23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>74</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2088,7 +2148,7 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="19"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
@@ -2116,7 +2176,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -2144,7 +2204,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="19"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -2172,7 +2232,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -2200,7 +2260,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
@@ -3152,7 +3212,7 @@
       <c r="Z79" s="1"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
@@ -29079,22 +29139,50 @@
       <c r="Y1005" s="1"/>
       <c r="Z1005" s="1"/>
     </row>
+    <row r="1006" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="3"/>
+      <c r="G1006" s="3"/>
+      <c r="H1006" s="3"/>
+      <c r="I1006" s="2"/>
+      <c r="J1006" s="3"/>
+      <c r="K1006" s="2"/>
+      <c r="L1006" s="3"/>
+      <c r="M1006" s="3"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E20:E1005 E1:E18" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E19 E21:E1006" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F20:F1005 F1:F18" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F19 F21:F1006" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C20:C50 C62:C1005 C1:C18" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C1:C19 C63:C1006 C21:C51" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H1005 H1:H18" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H19 H21:H1006" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -29158,7 +29246,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>13</v>

</xml_diff>